<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@f9c6bce8e85595c5b1bc22996569eb3c545e516b 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-collection-type-vs.xlsx
+++ b/ValueSet-collection-type-vs.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from Collection Type" r:id="rId4" sheetId="2"/>
+    <sheet name="Include #0" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-22T16:27:20+00:00</t>
+    <t>2024-09-10T18:56:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>